<commit_message>
Added start and end date of an issue to the output, changed the unit test accordingly
</commit_message>
<xml_diff>
--- a/test/excel_output.xlsx
+++ b/test/excel_output.xlsx
@@ -68,8 +68,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -137,8 +138,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -159,115 +168,136 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F3" activeCellId="0" sqref="F3"/>
+      <selection pane="topLeft" activeCell="H2" activeCellId="0" sqref="H2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="7" style="0" width="11.17"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="0" t="s">
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="0" t="s">
+      <c r="G1" s="2" t="n">
+        <v>43840</v>
+      </c>
+      <c r="H1" s="2" t="n">
+        <v>43845</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="0" t="s">
+      <c r="J1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="0" t="s">
+      <c r="K1" s="1" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="C2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="F2" s="0" t="s">
+      <c r="D2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="0" t="s">
+      <c r="G2" s="2" t="n">
+        <v>43840</v>
+      </c>
+      <c r="H2" s="2" t="n">
+        <v>43845</v>
+      </c>
+      <c r="I2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="0" t="s">
+      <c r="J2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="0" t="s">
+      <c r="K2" s="1" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="C3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="0" t="s">
+      <c r="D3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="F3" s="0" t="s">
+      <c r="E3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="0" t="s">
+      <c r="G3" s="2" t="n">
+        <v>43840</v>
+      </c>
+      <c r="H3" s="2" t="n">
+        <v>43845</v>
+      </c>
+      <c r="I3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H3" s="0" t="s">
+      <c r="J3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I3" s="0" t="s">
+      <c r="K3" s="1" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="0" t="s">
+      <c r="C4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="G4" s="0" t="s">
+      <c r="D4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="I4" s="1" t="s">
         <v>13</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Column header 'parent summary' fixed to 'parent_summary'. This way it is consistent with the other column names. Also fixed the excel unit test, the excel file was not generated before comparison.
</commit_message>
<xml_diff>
--- a/test/excel_output.xlsx
+++ b/test/excel_output.xlsx
@@ -52,7 +52,7 @@
     <t xml:space="preserve">parent</t>
   </si>
   <si>
-    <t xml:space="preserve">parent summary</t>
+    <t xml:space="preserve">parent_summary</t>
   </si>
   <si>
     <t xml:space="preserve">John Doe</t>
@@ -201,7 +201,7 @@
   <dimension ref="A1:K5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E5" activeCellId="0" sqref="E5"/>
+      <selection pane="topLeft" activeCell="K2" activeCellId="0" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>